<commit_message>
CHNM -> SAS in region code
</commit_message>
<xml_diff>
--- a/inst/extdata/test_data/FAO_ISO_MW_Mapping.xlsx
+++ b/inst/extdata/test_data/FAO_ISO_MW_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MWTools\inst\extdata\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F8E979-58F1-465E-9FA9-6BA4FF2EED70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC44720B-402D-4FB6-9859-5F4064ECE83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2211,7 +2211,7 @@
   <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2884,7 +2884,7 @@
         <v>460</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>458</v>

</xml_diff>